<commit_message>
Commited updated HomePage, Updated Organizations Page and OrganizationsExcelData
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/organizations.xlsx
+++ b/src/main/resources/excel/organizations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="TYC111973" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="TYC111954" sheetId="4" r:id="rId4"/>
     <sheet name="TYC121902" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,9 +22,146 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>TC No</t>
+  </si>
+  <si>
+    <t>TC Name</t>
+  </si>
+  <si>
+    <t>Alert Msg</t>
+  </si>
+  <si>
+    <t>VTIG-23</t>
+  </si>
+  <si>
+    <t>TC_021</t>
+  </si>
+  <si>
+    <t>DeleteFromOrganizationWithoutSlectinAnyOrganization</t>
+  </si>
+  <si>
+    <t>Please select at least one entity</t>
+  </si>
+  <si>
+    <t>OrgName</t>
+  </si>
+  <si>
+    <t>VTIG-21</t>
+  </si>
+  <si>
+    <t>TC_019</t>
+  </si>
+  <si>
+    <t>CancelThePopupDuringDeletionInAction</t>
+  </si>
+  <si>
+    <t>TestYantra</t>
+  </si>
+  <si>
+    <t>Are You Sure You want to Delete?</t>
+  </si>
+  <si>
+    <t>VTIG-20</t>
+  </si>
+  <si>
+    <t>TC_018</t>
+  </si>
+  <si>
+    <t>DeleteOrganizationFromAction</t>
+  </si>
+  <si>
+    <t>TYSS</t>
+  </si>
+  <si>
+    <t>VTIG-19</t>
+  </si>
+  <si>
+    <t>TC_017</t>
+  </si>
+  <si>
+    <t>CancelThePopupDuringMultipleDeletionInHeader</t>
+  </si>
+  <si>
+    <t>TYSS_QSP</t>
+  </si>
+  <si>
+    <t>Deleting this organization(s) will remove its related Opportunities &amp; Quotes. Are you sure you want to delete the selected</t>
+  </si>
+  <si>
+    <t>VTIG-18</t>
+  </si>
+  <si>
+    <t>TC_016</t>
+  </si>
+  <si>
+    <t>DeleteMultipleOrganizationFromHeader</t>
+  </si>
+  <si>
+    <t>TYSS_JSP</t>
+  </si>
+  <si>
+    <t>VTIG-17</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
+    <t>CancelThePopupDuringDeletionInHeader</t>
+  </si>
+  <si>
+    <t>TYSS_PSP</t>
+  </si>
+  <si>
+    <t>Deleting this organization(s) will remove its related Opportunities &amp; Quotes. Are you sure you want to delete the selected 1 records?</t>
+  </si>
+  <si>
+    <t>VTIG-16</t>
+  </si>
+  <si>
+    <t>TC_014</t>
+  </si>
+  <si>
+    <t>DeleteOrganizationFromHeader</t>
+  </si>
+  <si>
+    <t>TYSS_CSP</t>
+  </si>
+  <si>
+    <t>Billing Adress</t>
+  </si>
+  <si>
+    <t>VTIG-15</t>
+  </si>
+  <si>
+    <t>TC_013</t>
+  </si>
+  <si>
+    <t>CopyingAddressInformationToBillingAddress</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>VTIG-14</t>
+  </si>
+  <si>
+    <t>TC_012</t>
+  </si>
+  <si>
+    <t>CopyingAddressInformationToShippingAddress</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,15 +170,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -49,12 +192,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -327,67 +488,455 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="122" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="3" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" s="3" customFormat="1">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1">
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1">
+      <c r="A25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>